<commit_message>
added L:D as parameter
</commit_message>
<xml_diff>
--- a/R_data/Metadata_He028_PkVRF01.xlsx
+++ b/R_data/Metadata_He028_PkVRF01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofbergen-my.sharepoint.com/personal/marius_saltvedt_uib_no/Documents/PhD/2nd Work Package/Transcriptomics/2022_Krabberod_meeting/R_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofbergen-my.sharepoint.com/personal/marius_langvad_uib_no/Documents/PhD/2nd Work Package/Transcriptomics/VirVar-project_Transcriptomics/R_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{0126D0CD-C423-174B-9A97-AA29F78AF29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CB5A7F0-3FF0-D940-AA41-D50AF4E21D5C}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{0126D0CD-C423-174B-9A97-AA29F78AF29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93599791-5CA5-164D-ABE5-E0D8ADE67711}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{EFAD7797-2C0E-8442-B177-F520F12D1806}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14680" windowHeight="17940" xr2:uid="{EFAD7797-2C0E-8442-B177-F520F12D1806}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="163">
   <si>
     <t>Sample_name</t>
   </si>
@@ -516,12 +516,24 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>Dark_light</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -565,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,6 +589,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,9 +609,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -635,7 +649,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -741,7 +755,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -883,7 +897,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -893,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9B9E45-9F4B-C345-9050-7B29F7302621}">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -918,6 +932,9 @@
       <c r="E1" t="s">
         <v>156</v>
       </c>
+      <c r="F1" t="s">
+        <v>160</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
@@ -937,7 +954,11 @@
       <c r="E2" t="s">
         <v>150</v>
       </c>
+      <c r="F2" t="s">
+        <v>161</v>
+      </c>
       <c r="G2" s="2"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -955,7 +976,11 @@
       <c r="E3" t="s">
         <v>155</v>
       </c>
+      <c r="F3" t="s">
+        <v>161</v>
+      </c>
       <c r="G3" s="2"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -973,7 +998,11 @@
       <c r="E4" t="s">
         <v>153</v>
       </c>
+      <c r="F4" t="s">
+        <v>161</v>
+      </c>
       <c r="G4" s="2"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -991,7 +1020,11 @@
       <c r="E5" t="s">
         <v>150</v>
       </c>
+      <c r="F5" t="s">
+        <v>161</v>
+      </c>
       <c r="G5" s="2"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1009,7 +1042,11 @@
       <c r="E6" t="s">
         <v>155</v>
       </c>
+      <c r="F6" t="s">
+        <v>161</v>
+      </c>
       <c r="G6" s="2"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1027,7 +1064,11 @@
       <c r="E7" t="s">
         <v>153</v>
       </c>
+      <c r="F7" t="s">
+        <v>161</v>
+      </c>
       <c r="G7" s="2"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1045,7 +1086,11 @@
       <c r="E8" t="s">
         <v>155</v>
       </c>
+      <c r="F8" t="s">
+        <v>161</v>
+      </c>
       <c r="G8" s="2"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1063,7 +1108,11 @@
       <c r="E9" t="s">
         <v>153</v>
       </c>
+      <c r="F9" t="s">
+        <v>161</v>
+      </c>
       <c r="G9" s="2"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1081,7 +1130,11 @@
       <c r="E10" t="s">
         <v>150</v>
       </c>
+      <c r="F10" t="s">
+        <v>161</v>
+      </c>
       <c r="G10" s="2"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1099,6 +1152,9 @@
       <c r="E11" t="s">
         <v>155</v>
       </c>
+      <c r="F11" t="s">
+        <v>161</v>
+      </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1117,6 +1173,9 @@
       <c r="E12" t="s">
         <v>153</v>
       </c>
+      <c r="F12" t="s">
+        <v>161</v>
+      </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1135,6 +1194,9 @@
       <c r="E13" t="s">
         <v>150</v>
       </c>
+      <c r="F13" t="s">
+        <v>161</v>
+      </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1153,6 +1215,9 @@
       <c r="E14" t="s">
         <v>155</v>
       </c>
+      <c r="F14" t="s">
+        <v>161</v>
+      </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1171,6 +1236,9 @@
       <c r="E15" t="s">
         <v>153</v>
       </c>
+      <c r="F15" t="s">
+        <v>161</v>
+      </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1189,6 +1257,9 @@
       <c r="E16" t="s">
         <v>150</v>
       </c>
+      <c r="F16" t="s">
+        <v>161</v>
+      </c>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1207,6 +1278,9 @@
       <c r="E17" t="s">
         <v>155</v>
       </c>
+      <c r="F17" t="s">
+        <v>161</v>
+      </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1225,6 +1299,9 @@
       <c r="E18" t="s">
         <v>153</v>
       </c>
+      <c r="F18" t="s">
+        <v>161</v>
+      </c>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1243,6 +1320,9 @@
       <c r="E19" t="s">
         <v>150</v>
       </c>
+      <c r="F19" t="s">
+        <v>162</v>
+      </c>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1261,6 +1341,9 @@
       <c r="E20" t="s">
         <v>155</v>
       </c>
+      <c r="F20" t="s">
+        <v>162</v>
+      </c>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1279,6 +1362,9 @@
       <c r="E21" t="s">
         <v>153</v>
       </c>
+      <c r="F21" t="s">
+        <v>162</v>
+      </c>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1297,6 +1383,9 @@
       <c r="E22" t="s">
         <v>150</v>
       </c>
+      <c r="F22" t="s">
+        <v>162</v>
+      </c>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1315,6 +1404,9 @@
       <c r="E23" t="s">
         <v>155</v>
       </c>
+      <c r="F23" t="s">
+        <v>162</v>
+      </c>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1333,6 +1425,9 @@
       <c r="E24" t="s">
         <v>153</v>
       </c>
+      <c r="F24" t="s">
+        <v>162</v>
+      </c>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1351,6 +1446,9 @@
       <c r="E25" t="s">
         <v>150</v>
       </c>
+      <c r="F25" t="s">
+        <v>162</v>
+      </c>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1369,6 +1467,9 @@
       <c r="E26" t="s">
         <v>155</v>
       </c>
+      <c r="F26" t="s">
+        <v>162</v>
+      </c>
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1387,6 +1488,9 @@
       <c r="E27" t="s">
         <v>150</v>
       </c>
+      <c r="F27" t="s">
+        <v>162</v>
+      </c>
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1405,6 +1509,9 @@
       <c r="E28" t="s">
         <v>155</v>
       </c>
+      <c r="F28" t="s">
+        <v>162</v>
+      </c>
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1423,6 +1530,9 @@
       <c r="E29" t="s">
         <v>153</v>
       </c>
+      <c r="F29" t="s">
+        <v>162</v>
+      </c>
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1441,6 +1551,9 @@
       <c r="E30" t="s">
         <v>150</v>
       </c>
+      <c r="F30" t="s">
+        <v>162</v>
+      </c>
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1459,6 +1572,9 @@
       <c r="E31" t="s">
         <v>155</v>
       </c>
+      <c r="F31" t="s">
+        <v>162</v>
+      </c>
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1477,6 +1593,9 @@
       <c r="E32" t="s">
         <v>153</v>
       </c>
+      <c r="F32" t="s">
+        <v>162</v>
+      </c>
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1495,6 +1614,9 @@
       <c r="E33" t="s">
         <v>150</v>
       </c>
+      <c r="F33" t="s">
+        <v>162</v>
+      </c>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1513,6 +1635,9 @@
       <c r="E34" t="s">
         <v>155</v>
       </c>
+      <c r="F34" t="s">
+        <v>162</v>
+      </c>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1531,6 +1656,9 @@
       <c r="E35" t="s">
         <v>153</v>
       </c>
+      <c r="F35" t="s">
+        <v>162</v>
+      </c>
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1549,6 +1677,9 @@
       <c r="E36" t="s">
         <v>150</v>
       </c>
+      <c r="F36" t="s">
+        <v>162</v>
+      </c>
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1567,6 +1698,9 @@
       <c r="E37" t="s">
         <v>153</v>
       </c>
+      <c r="F37" t="s">
+        <v>162</v>
+      </c>
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1585,6 +1719,9 @@
       <c r="E38" t="s">
         <v>150</v>
       </c>
+      <c r="F38" t="s">
+        <v>161</v>
+      </c>
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1603,6 +1740,9 @@
       <c r="E39" t="s">
         <v>155</v>
       </c>
+      <c r="F39" t="s">
+        <v>161</v>
+      </c>
       <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1621,6 +1761,9 @@
       <c r="E40" t="s">
         <v>153</v>
       </c>
+      <c r="F40" t="s">
+        <v>161</v>
+      </c>
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1639,6 +1782,9 @@
       <c r="E41" t="s">
         <v>150</v>
       </c>
+      <c r="F41" t="s">
+        <v>161</v>
+      </c>
       <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1657,6 +1803,9 @@
       <c r="E42" t="s">
         <v>155</v>
       </c>
+      <c r="F42" t="s">
+        <v>161</v>
+      </c>
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1675,6 +1824,9 @@
       <c r="E43" t="s">
         <v>153</v>
       </c>
+      <c r="F43" t="s">
+        <v>161</v>
+      </c>
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1693,6 +1845,9 @@
       <c r="E44" t="s">
         <v>150</v>
       </c>
+      <c r="F44" t="s">
+        <v>161</v>
+      </c>
       <c r="G44" s="2"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1711,6 +1866,9 @@
       <c r="E45" t="s">
         <v>155</v>
       </c>
+      <c r="F45" t="s">
+        <v>161</v>
+      </c>
       <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1729,6 +1887,9 @@
       <c r="E46" t="s">
         <v>153</v>
       </c>
+      <c r="F46" t="s">
+        <v>161</v>
+      </c>
       <c r="G46" s="2"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1747,6 +1908,9 @@
       <c r="E47" t="s">
         <v>150</v>
       </c>
+      <c r="F47" t="s">
+        <v>161</v>
+      </c>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -1765,6 +1929,9 @@
       <c r="E48" t="s">
         <v>155</v>
       </c>
+      <c r="F48" t="s">
+        <v>161</v>
+      </c>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1783,6 +1950,9 @@
       <c r="E49" t="s">
         <v>153</v>
       </c>
+      <c r="F49" t="s">
+        <v>161</v>
+      </c>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1801,6 +1971,9 @@
       <c r="E50" t="s">
         <v>150</v>
       </c>
+      <c r="F50" t="s">
+        <v>161</v>
+      </c>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1819,6 +1992,9 @@
       <c r="E51" t="s">
         <v>155</v>
       </c>
+      <c r="F51" t="s">
+        <v>161</v>
+      </c>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1837,6 +2013,9 @@
       <c r="E52" t="s">
         <v>150</v>
       </c>
+      <c r="F52" t="s">
+        <v>162</v>
+      </c>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -1855,6 +2034,9 @@
       <c r="E53" t="s">
         <v>155</v>
       </c>
+      <c r="F53" t="s">
+        <v>162</v>
+      </c>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1873,6 +2055,9 @@
       <c r="E54" t="s">
         <v>153</v>
       </c>
+      <c r="F54" t="s">
+        <v>162</v>
+      </c>
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1891,6 +2076,9 @@
       <c r="E55" t="s">
         <v>150</v>
       </c>
+      <c r="F55" t="s">
+        <v>162</v>
+      </c>
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1909,6 +2097,9 @@
       <c r="E56" t="s">
         <v>155</v>
       </c>
+      <c r="F56" t="s">
+        <v>162</v>
+      </c>
       <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1927,6 +2118,9 @@
       <c r="E57" t="s">
         <v>153</v>
       </c>
+      <c r="F57" t="s">
+        <v>162</v>
+      </c>
       <c r="G57" s="2"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -1945,6 +2139,9 @@
       <c r="E58" t="s">
         <v>150</v>
       </c>
+      <c r="F58" t="s">
+        <v>162</v>
+      </c>
       <c r="G58" s="2"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -1963,6 +2160,9 @@
       <c r="E59" t="s">
         <v>155</v>
       </c>
+      <c r="F59" t="s">
+        <v>162</v>
+      </c>
       <c r="G59" s="2"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -1981,6 +2181,9 @@
       <c r="E60" t="s">
         <v>153</v>
       </c>
+      <c r="F60" t="s">
+        <v>162</v>
+      </c>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -1999,6 +2202,9 @@
       <c r="E61" t="s">
         <v>150</v>
       </c>
+      <c r="F61" t="s">
+        <v>162</v>
+      </c>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -2017,6 +2223,9 @@
       <c r="E62" t="s">
         <v>155</v>
       </c>
+      <c r="F62" t="s">
+        <v>162</v>
+      </c>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -2035,6 +2244,9 @@
       <c r="E63" t="s">
         <v>153</v>
       </c>
+      <c r="F63" t="s">
+        <v>162</v>
+      </c>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -2053,6 +2265,9 @@
       <c r="E64" t="s">
         <v>150</v>
       </c>
+      <c r="F64" t="s">
+        <v>161</v>
+      </c>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -2071,6 +2286,9 @@
       <c r="E65" t="s">
         <v>155</v>
       </c>
+      <c r="F65" t="s">
+        <v>161</v>
+      </c>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -2089,6 +2307,9 @@
       <c r="E66" t="s">
         <v>153</v>
       </c>
+      <c r="F66" t="s">
+        <v>161</v>
+      </c>
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -2107,6 +2328,9 @@
       <c r="E67" t="s">
         <v>150</v>
       </c>
+      <c r="F67" t="s">
+        <v>161</v>
+      </c>
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -2125,6 +2349,9 @@
       <c r="E68" t="s">
         <v>155</v>
       </c>
+      <c r="F68" t="s">
+        <v>161</v>
+      </c>
       <c r="G68" s="2"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -2143,6 +2370,9 @@
       <c r="E69" t="s">
         <v>153</v>
       </c>
+      <c r="F69" t="s">
+        <v>161</v>
+      </c>
       <c r="G69" s="2"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -2161,6 +2391,9 @@
       <c r="E70" t="s">
         <v>150</v>
       </c>
+      <c r="F70" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
@@ -2178,6 +2411,9 @@
       <c r="E71" t="s">
         <v>155</v>
       </c>
+      <c r="F71" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -2195,6 +2431,9 @@
       <c r="E72" t="s">
         <v>153</v>
       </c>
+      <c r="F72" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -2212,6 +2451,9 @@
       <c r="E73" t="s">
         <v>150</v>
       </c>
+      <c r="F73" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
@@ -2229,6 +2471,9 @@
       <c r="E74" t="s">
         <v>155</v>
       </c>
+      <c r="F74" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
@@ -2245,6 +2490,9 @@
       </c>
       <c r="E75" t="s">
         <v>153</v>
+      </c>
+      <c r="F75" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>